<commit_message>
Signed-off-by: Kiarash Behnam <kiarash@kth.se>
</commit_message>
<xml_diff>
--- a/Bank.xlsx
+++ b/Bank.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34958\Downloads\ONLINE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiarash\Desktop\ONLINE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6124778-0690-4106-B84E-D140DE1921EA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>lån</t>
   </si>
@@ -90,18 +91,26 @@
   </si>
   <si>
     <t>Hushåll per person</t>
+  </si>
+  <si>
+    <t>Sl</t>
+  </si>
+  <si>
+    <t>CSN</t>
+  </si>
+  <si>
+    <t>Fuck akassa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;kr&quot;_-;\-* #,##0\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +161,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -182,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -233,45 +258,159 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="4" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Accent5" xfId="5" builtinId="45"/>
-    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="5">
+    <cellStyle name="Anteckning" xfId="3" builtinId="10"/>
+    <cellStyle name="Beräkning" xfId="2" builtinId="22"/>
+    <cellStyle name="Dekorfärg5" xfId="4" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="4" builtinId="10"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -288,26 +427,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FFB2B2B2"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFB2B2B2"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFB2B2B2"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFB2B2B2"/>
-        </bottom>
-      </border>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;kr&quot;_-;\-* #,##0\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;kr&quot;_-;\-* #,##0\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -364,23 +504,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FFB2B2B2"/>
@@ -404,8 +527,35 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{3966F66B-86FE-4177-81C4-FECC42B408EB}">
+      <tableStyleElement type="wholeTable" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -418,11 +568,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A12:B26" totalsRowCount="1" dataDxfId="5" tableBorderDxfId="4" dataCellStyle="Note">
-  <autoFilter ref="A12:B25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B10:C24" totalsRowCount="1" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="B10:C23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="1" dataCellStyle="Note"/>
-    <tableColumn id="2" name="Kostnad" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="0" dataCellStyle="Note"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Kostnad" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Anteckning" totalsRowCellStyle="Anteckning"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -690,269 +840,298 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="0.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="G1" s="8" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20">
+        <v>4150000</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="W3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="X3" s="1">
+        <f>C3*W3</f>
+        <v>1245000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="20">
+        <v>500000</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="20">
+        <v>100000</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
+        <f>IF(C6&gt;0.5,0.01,IF(C6&gt;0.3,0.02,0.03))</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C6" s="6">
+        <f>(C4+C5)/C3</f>
+        <v>0.14457831325301204</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="22">
+        <v>4900</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="K1" s="8" t="s">
+      <c r="I11" s="14"/>
+      <c r="J11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="12">
-        <v>3500000</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="G3" t="s">
+    </row>
+    <row r="12" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="22">
+        <v>2000</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2">
-        <f>B3/2-B5</f>
-        <v>1650000</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="2">
-        <f>B3/2-B4</f>
-        <v>1250000</v>
-      </c>
-      <c r="U3" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="V3" s="2">
-        <f>B3*U3</f>
-        <v>1050000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="12">
-        <v>500000</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="13">
-        <v>0.02</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="G12" s="14"/>
+      <c r="H12" s="16">
+        <f>C3/2-C5</f>
+        <v>1975000</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="11">
+        <f>C3/2-C4</f>
+        <v>1575000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="22"/>
+      <c r="F13" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="1">
-        <f>H3*(D4+D5)</f>
-        <v>82500</v>
-      </c>
-      <c r="K4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="1">
-        <f>L3*(D4+D5)</f>
-        <v>62500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="12">
-        <v>100000</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="14">
-        <f>IF(B6&gt;0.5,0.01,IF(B6&gt;0.3,0.02,0.03))</f>
-        <v>0.03</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="G13" s="14"/>
+      <c r="H13" s="17">
+        <f>H12*(E4+E5)</f>
+        <v>98750</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="12">
+        <f>J12*(E4+E5)</f>
+        <v>78750</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="22">
+        <v>4000</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="1">
-        <f>H4/12</f>
-        <v>6875</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="1">
-        <f>L4/12</f>
-        <v>5208.333333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B6" s="9">
-        <f>(B4+B5)/B3</f>
-        <v>0.17142857142857143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="G7" t="s">
+      <c r="G14" s="14"/>
+      <c r="H14" s="17">
+        <f>H13/12</f>
+        <v>8229.1666666666661</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="12">
+        <f>J13/12</f>
+        <v>6562.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="22">
+        <v>3000</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="22">
+        <v>3000</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="1">
+      <c r="G16" s="14"/>
+      <c r="H16" s="17">
         <f>Table1[[#Totals],[Kostnad]]/2</f>
-        <v>9000</v>
-      </c>
-      <c r="K7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="1">
+        <v>11250</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="12">
         <f>Table1[[#Totals],[Kostnad]]/2</f>
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="22">
+        <v>2000</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="22">
+        <v>800</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="22">
+        <v>1800</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="22">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="13"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="23"/>
+      <c r="C21" s="22"/>
+      <c r="F21" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="1">
-        <f>Table1[[#Totals],[Kostnad]]/2+H5</f>
-        <v>15875</v>
-      </c>
-      <c r="K12" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12" s="2">
-        <f>Table1[[#Totals],[Kostnad]]/2+L5</f>
-        <v>14208.333333333332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="5">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
+      <c r="G21" s="14"/>
+      <c r="H21" s="17">
+        <f>Table1[[#Totals],[Kostnad]]/2+H14</f>
+        <v>19479.166666666664</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="12">
+        <f>Table1[[#Totals],[Kostnad]]/2+J14</f>
+        <v>17812.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="23"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="24"/>
+      <c r="C23" s="22"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="7">
+      <c r="C24" s="4">
         <f>SUBTOTAL(109,Table1[Kostnad])</f>
-        <v>18000</v>
+        <v>22500</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A2:D2"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Ada2Pb7wsIaOGH/J0XsvfxzmIg9U+3n2gXpBEvi6VeSdHuBh1QgvIpVtip7U2ogp+o8OGRYgnxL/Bfc9ZfQbhw==" saltValue="cBFlRqvCRoA7b9BN+DoEbA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>